<commit_message>
davco 65+ initial commit
</commit_message>
<xml_diff>
--- a/2. Senior Centers MySidewalk Profiles/Links.xlsx
+++ b/2. Senior Centers MySidewalk Profiles/Links.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmccall\Documents\GIT\Aging-and-Disability\Senior Centers MySidewalk Profiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmccall\Documents\GIT\Aging-and-Disability\2. Senior Centers MySidewalk Profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B93AA9AE-A2EC-489D-8C58-E832B6265A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC63234-E32A-4374-8F20-9DA38CF60BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1CD0229A-F620-4196-AA79-56E31D946D52}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1CD0229A-F620-4196-AA79-56E31D946D52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>Center</t>
   </si>
@@ -185,6 +185,12 @@
   </si>
   <si>
     <t>https://reports.mysidewalk.com/1f9c415316</t>
+  </si>
+  <si>
+    <t>https://reports.mysidewalk.com/b797651eb3</t>
+  </si>
+  <si>
+    <t>FiftyForward Madison Station Senior Center</t>
   </si>
 </sst>
 </file>
@@ -547,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD2A5125-F05F-4D1D-AAFE-5C491906A55D}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,6 +762,17 @@
       </c>
       <c r="C18" s="1" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -777,6 +794,7 @@
     <hyperlink ref="C15" r:id="rId15" xr:uid="{8284599C-BA1B-4AE4-85A1-E600BDBFC858}"/>
     <hyperlink ref="C17" r:id="rId16" xr:uid="{6FA9DDB7-5C7A-4AF3-B33D-BB614332B76F}"/>
     <hyperlink ref="C18" r:id="rId17" xr:uid="{3A7FD78F-3FD1-4CD0-B1DE-19219398B17A}"/>
+    <hyperlink ref="C19" r:id="rId18" xr:uid="{BEF94B51-8B95-49C6-9B0F-F79AC033037B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>